<commit_message>
update some knowledge docs
</commit_message>
<xml_diff>
--- a/SKWIN/knowledge/Skulldat.xlsx
+++ b/SKWIN/knowledge/Skulldat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="312" windowWidth="11340" windowHeight="6348" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="312" windowWidth="11340" windowHeight="6348"/>
   </bookViews>
   <sheets>
     <sheet name="skull" sheetId="1" r:id="rId1"/>
@@ -113,15 +113,6 @@
   </si>
   <si>
     <t>B23</t>
-  </si>
-  <si>
-    <t>FIRE RES</t>
-  </si>
-  <si>
-    <t>B25</t>
-  </si>
-  <si>
-    <t>POISON RES</t>
   </si>
   <si>
     <t>B26</t>
@@ -319,9 +310,6 @@
     <t>#id</t>
   </si>
   <si>
-    <t>B24 (FEAR?)</t>
-  </si>
-  <si>
     <t>ACTIVATE PIT/TELEPORT (0x40)</t>
   </si>
   <si>
@@ -446,6 +434,21 @@
   </si>
   <si>
     <t>Cavern / Stone Table / Wall Hole</t>
+  </si>
+  <si>
+    <t>B25 LOW
+POISON RES</t>
+  </si>
+  <si>
+    <t>B25 HIGH</t>
+  </si>
+  <si>
+    <t>B24 LOW
+(FEAR?)</t>
+  </si>
+  <si>
+    <t>B24 HIGH
+FIRE RES</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1045,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1076,6 +1079,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1491,11 +1497,11 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:BK65"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X37" sqref="X37"/>
+      <selection pane="bottomRight" activeCell="AX1" sqref="AX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -1507,15 +1513,15 @@
     <col min="13" max="20" width="2.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="18.75" customHeight="1">
+    <row r="1" spans="1:63" ht="45.6" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1545,28 +1551,28 @@
         <v>9</v>
       </c>
       <c r="M1" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q1" t="s">
         <v>107</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>108</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
         <v>109</v>
       </c>
-      <c r="P1" t="s">
+      <c r="T1" t="s">
         <v>110</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>111</v>
-      </c>
-      <c r="R1" t="s">
-        <v>112</v>
-      </c>
-      <c r="S1" t="s">
-        <v>113</v>
-      </c>
-      <c r="T1" t="s">
-        <v>114</v>
       </c>
       <c r="U1" t="s">
         <v>10</v>
@@ -1590,25 +1596,25 @@
         <v>16</v>
       </c>
       <c r="AB1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF1" t="s">
         <v>100</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AG1" t="s">
         <v>101</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AH1" t="s">
         <v>102</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>106</v>
       </c>
       <c r="AI1" t="s">
         <v>17</v>
@@ -1652,52 +1658,52 @@
       <c r="AV1" t="s">
         <v>30</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AW1" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="AX1" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AZ1" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="BA1" t="s">
         <v>31</v>
       </c>
-      <c r="AX1" t="s">
-        <v>99</v>
-      </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>32</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" t="s">
         <v>33</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>34</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BE1" t="s">
         <v>35</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BF1" t="s">
         <v>36</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BG1" t="s">
         <v>37</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BH1" t="s">
         <v>38</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BI1" t="s">
         <v>39</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BJ1" t="s">
         <v>40</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>41</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>42</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:63">
       <c r="A2" s="29" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B2" s="29">
         <v>0</v>
@@ -1869,7 +1875,7 @@
     </row>
     <row r="3" spans="1:63" s="3" customFormat="1">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -2034,7 +2040,7 @@
     </row>
     <row r="4" spans="1:63" s="3" customFormat="1">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2">
         <v>3</v>
@@ -2199,7 +2205,7 @@
     </row>
     <row r="5" spans="1:63" s="3" customFormat="1">
       <c r="A5" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B5" s="2">
         <v>4</v>
@@ -2364,7 +2370,7 @@
     </row>
     <row r="6" spans="1:63" s="3" customFormat="1">
       <c r="A6" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B6" s="2">
         <v>5</v>
@@ -2529,7 +2535,7 @@
     </row>
     <row r="7" spans="1:63" s="3" customFormat="1">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -2694,7 +2700,7 @@
     </row>
     <row r="8" spans="1:63" s="3" customFormat="1">
       <c r="A8" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2">
         <v>7</v>
@@ -2859,7 +2865,7 @@
     </row>
     <row r="9" spans="1:63" s="3" customFormat="1">
       <c r="A9" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B9" s="2">
         <v>8</v>
@@ -3024,7 +3030,7 @@
     </row>
     <row r="10" spans="1:63" s="3" customFormat="1">
       <c r="A10" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B10" s="2">
         <v>9</v>
@@ -3189,7 +3195,7 @@
     </row>
     <row r="11" spans="1:63" s="3" customFormat="1">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2">
         <v>10</v>
@@ -3354,7 +3360,7 @@
     </row>
     <row r="12" spans="1:63" s="3" customFormat="1">
       <c r="A12" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B12" s="2">
         <v>11</v>
@@ -3519,7 +3525,7 @@
     </row>
     <row r="13" spans="1:63" s="3" customFormat="1">
       <c r="A13" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B13" s="2">
         <v>12</v>
@@ -3684,7 +3690,7 @@
     </row>
     <row r="14" spans="1:63" s="3" customFormat="1">
       <c r="A14" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B14" s="4">
         <v>13</v>
@@ -3865,7 +3871,7 @@
     </row>
     <row r="15" spans="1:63" s="5" customFormat="1">
       <c r="A15" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B15" s="4">
         <v>14</v>
@@ -4039,7 +4045,7 @@
     </row>
     <row r="16" spans="1:63" s="5" customFormat="1">
       <c r="A16" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B16" s="4">
         <v>15</v>
@@ -4213,7 +4219,7 @@
     </row>
     <row r="17" spans="1:63" s="5" customFormat="1">
       <c r="A17" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B17" s="4">
         <v>16</v>
@@ -4387,7 +4393,7 @@
     </row>
     <row r="18" spans="1:63" s="5" customFormat="1">
       <c r="A18" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B18" s="4">
         <v>17</v>
@@ -4561,7 +4567,7 @@
     </row>
     <row r="19" spans="1:63" s="11" customFormat="1">
       <c r="A19" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B19" s="4">
         <v>18</v>
@@ -4740,7 +4746,7 @@
     </row>
     <row r="20" spans="1:63" s="5" customFormat="1">
       <c r="A20" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B20" s="6">
         <v>19</v>
@@ -4915,7 +4921,7 @@
     </row>
     <row r="21" spans="1:63" s="7" customFormat="1">
       <c r="A21" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B21" s="2">
         <v>20</v>
@@ -5090,7 +5096,7 @@
     </row>
     <row r="22" spans="1:63" s="3" customFormat="1">
       <c r="A22" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B22" s="6">
         <v>21</v>
@@ -5269,7 +5275,7 @@
     </row>
     <row r="23" spans="1:63" s="7" customFormat="1">
       <c r="A23" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="6">
         <v>22</v>
@@ -5440,7 +5446,7 @@
     </row>
     <row r="24" spans="1:63" s="7" customFormat="1">
       <c r="A24" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B24" s="6">
         <v>23</v>
@@ -5611,7 +5617,7 @@
     </row>
     <row r="25" spans="1:63" s="7" customFormat="1">
       <c r="A25" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B25" s="6">
         <v>24</v>
@@ -5782,7 +5788,7 @@
     </row>
     <row r="26" spans="1:63" s="7" customFormat="1">
       <c r="A26" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B26" s="6">
         <v>25</v>
@@ -5953,7 +5959,7 @@
     </row>
     <row r="27" spans="1:63" s="7" customFormat="1">
       <c r="A27" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B27" s="6">
         <v>26</v>
@@ -6121,7 +6127,7 @@
     </row>
     <row r="28" spans="1:63" s="7" customFormat="1">
       <c r="A28" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B28" s="6">
         <v>27</v>
@@ -6289,7 +6295,7 @@
     </row>
     <row r="29" spans="1:63" s="7" customFormat="1">
       <c r="A29" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B29" s="6">
         <v>28</v>
@@ -6460,7 +6466,7 @@
     </row>
     <row r="30" spans="1:63" s="7" customFormat="1">
       <c r="A30" s="6" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B30" s="6">
         <v>29</v>
@@ -6631,7 +6637,7 @@
     </row>
     <row r="31" spans="1:63" s="7" customFormat="1">
       <c r="A31" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B31" s="6">
         <v>30</v>
@@ -6805,7 +6811,7 @@
     </row>
     <row r="32" spans="1:63" s="7" customFormat="1">
       <c r="A32" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B32" s="6">
         <v>31</v>
@@ -6970,7 +6976,7 @@
     </row>
     <row r="33" spans="1:63" s="7" customFormat="1">
       <c r="A33" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B33" s="2">
         <v>32</v>
@@ -7143,7 +7149,7 @@
     </row>
     <row r="34" spans="1:63" s="3" customFormat="1">
       <c r="A34" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B34" s="6">
         <v>33</v>
@@ -7318,7 +7324,7 @@
     </row>
     <row r="35" spans="1:63" s="7" customFormat="1">
       <c r="A35" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B35" s="6">
         <v>35</v>
@@ -7489,7 +7495,7 @@
     </row>
     <row r="36" spans="1:63">
       <c r="A36" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B36" s="6">
         <v>36</v>
@@ -7663,7 +7669,7 @@
     </row>
     <row r="37" spans="1:63" s="7" customFormat="1">
       <c r="A37" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B37" s="2">
         <v>37</v>
@@ -7836,7 +7842,7 @@
     </row>
     <row r="38" spans="1:63" s="7" customFormat="1">
       <c r="A38" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B38" s="2">
         <v>38</v>
@@ -8009,7 +8015,7 @@
     </row>
     <row r="39" spans="1:63" s="3" customFormat="1">
       <c r="A39" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B39" s="2">
         <v>39</v>
@@ -8174,7 +8180,7 @@
     </row>
     <row r="40" spans="1:63" s="3" customFormat="1">
       <c r="A40" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B40" s="2">
         <v>40</v>
@@ -8342,7 +8348,7 @@
     </row>
     <row r="41" spans="1:63" s="3" customFormat="1">
       <c r="A41" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B41" s="8">
         <v>41</v>
@@ -8521,7 +8527,7 @@
     </row>
     <row r="42" spans="1:63" s="3" customFormat="1">
       <c r="A42" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B42" s="6">
         <v>42</v>
@@ -8696,7 +8702,7 @@
     </row>
     <row r="43" spans="1:63" s="9" customFormat="1">
       <c r="A43" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B43" s="4">
         <v>43</v>
@@ -8875,7 +8881,7 @@
     </row>
     <row r="44" spans="1:63" s="7" customFormat="1">
       <c r="A44" s="6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B44" s="6">
         <v>44</v>
@@ -9043,7 +9049,7 @@
     </row>
     <row r="45" spans="1:63" s="5" customFormat="1">
       <c r="A45" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B45" s="2">
         <v>45</v>
@@ -9216,7 +9222,7 @@
     </row>
     <row r="46" spans="1:63" s="7" customFormat="1">
       <c r="A46" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B46" s="6">
         <v>46</v>
@@ -9384,7 +9390,7 @@
     </row>
     <row r="47" spans="1:63" s="3" customFormat="1">
       <c r="A47" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B47" s="2">
         <v>47</v>
@@ -9552,7 +9558,7 @@
     </row>
     <row r="48" spans="1:63" s="7" customFormat="1">
       <c r="A48" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B48" s="6">
         <v>48</v>
@@ -9720,7 +9726,7 @@
     </row>
     <row r="49" spans="1:63" s="3" customFormat="1">
       <c r="A49" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B49" s="4">
         <v>49</v>
@@ -9899,7 +9905,7 @@
     </row>
     <row r="50" spans="1:63" s="7" customFormat="1">
       <c r="A50" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B50" s="6">
         <v>50</v>
@@ -10067,7 +10073,7 @@
     </row>
     <row r="51" spans="1:63" s="5" customFormat="1">
       <c r="A51" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B51" s="2">
         <v>51</v>
@@ -10240,7 +10246,7 @@
     </row>
     <row r="52" spans="1:63" s="7" customFormat="1">
       <c r="A52" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B52" s="6">
         <v>52</v>
@@ -10408,7 +10414,7 @@
     </row>
     <row r="53" spans="1:63" s="3" customFormat="1">
       <c r="A53" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B53" s="10">
         <v>53</v>
@@ -10589,7 +10595,7 @@
     </row>
     <row r="54" spans="1:63" s="7" customFormat="1">
       <c r="A54" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B54" s="1">
         <v>54</v>
@@ -10769,7 +10775,7 @@
     </row>
     <row r="55" spans="1:63" s="7" customFormat="1">
       <c r="A55" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B55" s="6">
         <v>55</v>
@@ -10937,7 +10943,7 @@
     </row>
     <row r="56" spans="1:63">
       <c r="A56" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B56" s="1">
         <v>56</v>
@@ -11104,7 +11110,7 @@
     </row>
     <row r="57" spans="1:63" s="7" customFormat="1">
       <c r="A57" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B57" s="6">
         <v>57</v>
@@ -11272,7 +11278,7 @@
     </row>
     <row r="58" spans="1:63">
       <c r="A58" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B58" s="6">
         <v>58</v>
@@ -11446,7 +11452,7 @@
     </row>
     <row r="59" spans="1:63" s="7" customFormat="1">
       <c r="A59" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B59" s="2">
         <v>59</v>
@@ -11619,7 +11625,7 @@
     </row>
     <row r="60" spans="1:63" s="7" customFormat="1">
       <c r="A60" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B60" s="2">
         <v>60</v>
@@ -11792,7 +11798,7 @@
     </row>
     <row r="61" spans="1:63" s="3" customFormat="1">
       <c r="A61" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B61" s="8">
         <v>61</v>
@@ -11970,171 +11976,195 @@
       <c r="BK61"/>
     </row>
     <row r="62" spans="1:63" s="3" customFormat="1">
-      <c r="A62" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2">
-        <v>46</v>
-      </c>
-      <c r="D62" s="3">
-        <v>1</v>
-      </c>
-      <c r="E62" s="3">
-        <v>0</v>
-      </c>
-      <c r="F62" s="3">
-        <v>0</v>
-      </c>
-      <c r="G62" s="3">
-        <v>0</v>
-      </c>
-      <c r="H62" s="3">
-        <v>0</v>
-      </c>
-      <c r="I62" s="3">
-        <v>1</v>
-      </c>
-      <c r="J62" s="3">
-        <v>0</v>
-      </c>
-      <c r="K62" s="3">
-        <v>1</v>
-      </c>
-      <c r="L62" s="3">
-        <v>0</v>
-      </c>
-      <c r="U62" s="13">
+      <c r="A62" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1">
+        <v>37</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62">
         <v>255</v>
       </c>
-      <c r="V62" s="3">
-        <v>0</v>
-      </c>
-      <c r="W62" s="3">
-        <v>100</v>
-      </c>
-      <c r="X62" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y62" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z62" s="13">
-        <v>255</v>
-      </c>
-      <c r="AA62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AG62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AH62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AI62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AJ62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AO62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AQ62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AR62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AS62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AT62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AU62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AV62" s="3">
-        <v>1</v>
-      </c>
-      <c r="AW62" s="16">
-        <v>15</v>
-      </c>
-      <c r="AX62" s="17">
-        <v>15</v>
-      </c>
-      <c r="AY62" s="3">
-        <v>0</v>
-      </c>
-      <c r="AZ62" s="9">
-        <v>15</v>
-      </c>
-      <c r="BA62" s="3">
-        <v>0</v>
-      </c>
-      <c r="BB62" s="3">
-        <v>240</v>
-      </c>
-      <c r="BC62" s="3">
-        <v>0</v>
-      </c>
-      <c r="BD62" s="13">
-        <v>255</v>
-      </c>
-      <c r="BE62" s="3">
-        <v>34</v>
-      </c>
-      <c r="BF62" s="3">
-        <v>158</v>
-      </c>
-      <c r="BG62" s="3">
-        <v>20</v>
-      </c>
-      <c r="BH62" s="3">
-        <v>16</v>
-      </c>
-      <c r="BI62" s="3">
-        <v>0</v>
-      </c>
-      <c r="BJ62" s="3">
-        <v>2</v>
+      <c r="M62">
+        <v>1</v>
+      </c>
+      <c r="N62">
+        <v>1</v>
+      </c>
+      <c r="O62">
+        <v>1</v>
+      </c>
+      <c r="P62">
+        <v>1</v>
+      </c>
+      <c r="Q62">
+        <v>1</v>
+      </c>
+      <c r="R62">
+        <v>1</v>
+      </c>
+      <c r="S62">
+        <v>1</v>
+      </c>
+      <c r="T62">
+        <v>1</v>
+      </c>
+      <c r="U62">
+        <v>6</v>
+      </c>
+      <c r="V62">
+        <v>0</v>
+      </c>
+      <c r="W62">
+        <v>256</v>
+      </c>
+      <c r="X62">
+        <v>1</v>
+      </c>
+      <c r="Y62">
+        <v>0</v>
+      </c>
+      <c r="Z62">
+        <v>1</v>
+      </c>
+      <c r="AA62">
+        <v>0</v>
+      </c>
+      <c r="AB62">
+        <v>0</v>
+      </c>
+      <c r="AC62">
+        <v>0</v>
+      </c>
+      <c r="AD62">
+        <v>0</v>
+      </c>
+      <c r="AE62">
+        <v>0</v>
+      </c>
+      <c r="AF62">
+        <v>0</v>
+      </c>
+      <c r="AG62">
+        <v>0</v>
+      </c>
+      <c r="AH62">
+        <v>0</v>
+      </c>
+      <c r="AI62">
+        <v>0</v>
+      </c>
+      <c r="AJ62">
+        <v>1</v>
+      </c>
+      <c r="AK62">
+        <v>0</v>
+      </c>
+      <c r="AL62">
+        <v>1</v>
+      </c>
+      <c r="AM62">
+        <v>0</v>
+      </c>
+      <c r="AN62">
+        <v>0</v>
+      </c>
+      <c r="AO62">
+        <v>0</v>
+      </c>
+      <c r="AP62">
+        <v>0</v>
+      </c>
+      <c r="AQ62">
+        <v>0</v>
+      </c>
+      <c r="AR62">
+        <v>0</v>
+      </c>
+      <c r="AS62">
+        <v>0</v>
+      </c>
+      <c r="AT62">
+        <v>0</v>
+      </c>
+      <c r="AU62">
+        <v>0</v>
+      </c>
+      <c r="AV62">
+        <v>0</v>
+      </c>
+      <c r="AW62">
+        <v>0</v>
+      </c>
+      <c r="AX62">
+        <v>0</v>
+      </c>
+      <c r="AY62">
+        <v>0</v>
+      </c>
+      <c r="AZ62">
+        <v>0</v>
+      </c>
+      <c r="BA62">
+        <v>0</v>
+      </c>
+      <c r="BB62">
+        <v>0</v>
+      </c>
+      <c r="BC62">
+        <v>0</v>
+      </c>
+      <c r="BD62">
+        <v>0</v>
+      </c>
+      <c r="BE62">
+        <v>1</v>
+      </c>
+      <c r="BF62">
+        <v>0</v>
+      </c>
+      <c r="BG62">
+        <v>0</v>
+      </c>
+      <c r="BH62">
+        <v>0</v>
+      </c>
+      <c r="BI62">
+        <v>0</v>
+      </c>
+      <c r="BJ62">
+        <v>0</v>
       </c>
       <c r="BK62"/>
     </row>
     <row r="63" spans="1:63" s="9" customFormat="1">
       <c r="A63" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1">
@@ -12311,172 +12341,157 @@
     </row>
     <row r="64" spans="1:63">
       <c r="A64" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C64" s="1">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64">
         <v>1</v>
       </c>
       <c r="F64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L64">
+        <v>200</v>
+      </c>
+      <c r="P64" s="5">
+        <v>1</v>
+      </c>
+      <c r="S64" s="5">
+        <v>1</v>
+      </c>
+      <c r="T64" s="5">
+        <v>1</v>
+      </c>
+      <c r="U64">
+        <v>75</v>
+      </c>
+      <c r="V64">
+        <v>8</v>
+      </c>
+      <c r="W64">
+        <v>300</v>
+      </c>
+      <c r="X64">
+        <v>45</v>
+      </c>
+      <c r="Y64">
+        <v>0</v>
+      </c>
+      <c r="Z64">
+        <v>180</v>
+      </c>
+      <c r="AA64">
+        <v>0</v>
+      </c>
+      <c r="AB64">
+        <v>0</v>
+      </c>
+      <c r="AC64">
+        <v>0</v>
+      </c>
+      <c r="AD64" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE64" s="19">
+        <v>1</v>
+      </c>
+      <c r="AF64" s="20">
+        <v>1</v>
+      </c>
+      <c r="AG64">
+        <v>0</v>
+      </c>
+      <c r="AH64">
+        <v>0</v>
+      </c>
+      <c r="AI64">
+        <v>158</v>
+      </c>
+      <c r="AJ64">
+        <v>109</v>
+      </c>
+      <c r="AK64">
+        <v>0</v>
+      </c>
+      <c r="AL64">
+        <v>0</v>
+      </c>
+      <c r="AM64">
+        <v>64</v>
+      </c>
+      <c r="AN64">
+        <v>0</v>
+      </c>
+      <c r="AO64">
+        <v>33</v>
+      </c>
+      <c r="AP64">
+        <v>0</v>
+      </c>
+      <c r="AQ64">
+        <v>0</v>
+      </c>
+      <c r="AR64">
+        <v>0</v>
+      </c>
+      <c r="AS64">
         <v>255</v>
       </c>
-      <c r="M64">
-        <v>1</v>
-      </c>
-      <c r="N64">
-        <v>1</v>
-      </c>
-      <c r="O64">
-        <v>1</v>
-      </c>
-      <c r="P64">
-        <v>1</v>
-      </c>
-      <c r="Q64">
-        <v>1</v>
-      </c>
-      <c r="R64">
-        <v>1</v>
-      </c>
-      <c r="S64">
-        <v>1</v>
-      </c>
-      <c r="T64">
-        <v>1</v>
-      </c>
-      <c r="U64">
-        <v>6</v>
-      </c>
-      <c r="V64">
-        <v>0</v>
-      </c>
-      <c r="W64">
-        <v>256</v>
-      </c>
-      <c r="X64">
-        <v>1</v>
-      </c>
-      <c r="Y64">
-        <v>0</v>
-      </c>
-      <c r="Z64">
-        <v>1</v>
-      </c>
-      <c r="AA64">
-        <v>0</v>
-      </c>
-      <c r="AB64">
-        <v>0</v>
-      </c>
-      <c r="AC64">
-        <v>0</v>
-      </c>
-      <c r="AD64">
-        <v>0</v>
-      </c>
-      <c r="AE64">
-        <v>0</v>
-      </c>
-      <c r="AF64">
-        <v>0</v>
-      </c>
-      <c r="AG64">
-        <v>0</v>
-      </c>
-      <c r="AH64">
-        <v>0</v>
-      </c>
-      <c r="AI64">
-        <v>0</v>
-      </c>
-      <c r="AJ64">
-        <v>1</v>
-      </c>
-      <c r="AK64">
-        <v>0</v>
-      </c>
-      <c r="AL64">
-        <v>1</v>
-      </c>
-      <c r="AM64">
-        <v>0</v>
-      </c>
-      <c r="AN64">
-        <v>0</v>
-      </c>
-      <c r="AO64">
-        <v>0</v>
-      </c>
-      <c r="AP64">
-        <v>0</v>
-      </c>
-      <c r="AQ64">
-        <v>0</v>
-      </c>
-      <c r="AR64">
-        <v>0</v>
-      </c>
-      <c r="AS64">
-        <v>0</v>
-      </c>
       <c r="AT64">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="AU64">
-        <v>0</v>
+        <v>236</v>
       </c>
       <c r="AV64">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AW64">
-        <v>0</v>
-      </c>
-      <c r="AX64">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="AX64" s="17">
+        <v>15</v>
       </c>
       <c r="AY64">
         <v>0</v>
       </c>
       <c r="AZ64">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="BA64">
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="BB64">
-        <v>0</v>
+        <v>252</v>
       </c>
       <c r="BC64">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BD64">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="BE64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF64">
         <v>0</v>
@@ -12491,177 +12506,177 @@
         <v>0</v>
       </c>
       <c r="BJ64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:62">
-      <c r="A65" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C65" s="1">
-        <v>28</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-      <c r="E65">
-        <v>1</v>
-      </c>
-      <c r="F65">
-        <v>0</v>
-      </c>
-      <c r="G65">
-        <v>0</v>
-      </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
-      <c r="I65">
-        <v>0</v>
-      </c>
-      <c r="J65">
-        <v>0</v>
-      </c>
-      <c r="K65">
-        <v>0</v>
-      </c>
-      <c r="L65">
-        <v>200</v>
-      </c>
-      <c r="P65" s="5">
-        <v>1</v>
-      </c>
-      <c r="S65" s="5">
-        <v>1</v>
-      </c>
-      <c r="T65" s="5">
-        <v>1</v>
-      </c>
-      <c r="U65">
-        <v>75</v>
-      </c>
-      <c r="V65">
-        <v>8</v>
-      </c>
-      <c r="W65">
-        <v>300</v>
-      </c>
-      <c r="X65">
-        <v>45</v>
-      </c>
-      <c r="Y65">
-        <v>0</v>
-      </c>
-      <c r="Z65">
-        <v>180</v>
-      </c>
-      <c r="AA65">
-        <v>0</v>
-      </c>
-      <c r="AB65">
-        <v>0</v>
-      </c>
-      <c r="AC65">
-        <v>0</v>
-      </c>
-      <c r="AD65" s="15">
-        <v>1</v>
-      </c>
-      <c r="AE65" s="19">
-        <v>1</v>
-      </c>
-      <c r="AF65" s="20">
-        <v>1</v>
-      </c>
-      <c r="AG65">
-        <v>0</v>
-      </c>
-      <c r="AH65">
-        <v>0</v>
-      </c>
-      <c r="AI65">
-        <v>158</v>
-      </c>
-      <c r="AJ65">
-        <v>109</v>
-      </c>
-      <c r="AK65">
-        <v>0</v>
-      </c>
-      <c r="AL65">
-        <v>0</v>
-      </c>
-      <c r="AM65">
-        <v>64</v>
-      </c>
-      <c r="AN65">
-        <v>0</v>
-      </c>
-      <c r="AO65">
-        <v>33</v>
-      </c>
-      <c r="AP65">
-        <v>0</v>
-      </c>
-      <c r="AQ65">
-        <v>0</v>
-      </c>
-      <c r="AR65">
-        <v>0</v>
-      </c>
-      <c r="AS65">
+      <c r="A65" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2">
+        <v>46</v>
+      </c>
+      <c r="D65" s="3">
+        <v>1</v>
+      </c>
+      <c r="E65" s="3">
+        <v>0</v>
+      </c>
+      <c r="F65" s="3">
+        <v>0</v>
+      </c>
+      <c r="G65" s="3">
+        <v>0</v>
+      </c>
+      <c r="H65" s="3">
+        <v>0</v>
+      </c>
+      <c r="I65" s="3">
+        <v>1</v>
+      </c>
+      <c r="J65" s="3">
+        <v>0</v>
+      </c>
+      <c r="K65" s="3">
+        <v>1</v>
+      </c>
+      <c r="L65" s="3">
+        <v>0</v>
+      </c>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="3"/>
+      <c r="T65" s="3"/>
+      <c r="U65" s="13">
         <v>255</v>
       </c>
-      <c r="AT65">
-        <v>32</v>
-      </c>
-      <c r="AU65">
-        <v>236</v>
-      </c>
-      <c r="AV65">
-        <v>3</v>
-      </c>
-      <c r="AW65">
-        <v>7</v>
+      <c r="V65" s="3">
+        <v>0</v>
+      </c>
+      <c r="W65" s="3">
+        <v>100</v>
+      </c>
+      <c r="X65" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y65" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="13">
+        <v>255</v>
+      </c>
+      <c r="AA65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AJ65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AK65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AL65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AN65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AO65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AP65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AR65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AS65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AT65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AU65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AV65" s="3">
+        <v>1</v>
+      </c>
+      <c r="AW65" s="16">
+        <v>15</v>
       </c>
       <c r="AX65" s="17">
         <v>15</v>
       </c>
-      <c r="AY65">
-        <v>0</v>
-      </c>
-      <c r="AZ65">
-        <v>12</v>
-      </c>
-      <c r="BA65">
-        <v>160</v>
-      </c>
-      <c r="BB65">
-        <v>252</v>
-      </c>
-      <c r="BC65">
-        <v>4</v>
-      </c>
-      <c r="BD65">
-        <v>10</v>
-      </c>
-      <c r="BE65">
-        <v>0</v>
-      </c>
-      <c r="BF65">
-        <v>0</v>
-      </c>
-      <c r="BG65">
-        <v>0</v>
-      </c>
-      <c r="BH65">
-        <v>0</v>
-      </c>
-      <c r="BI65">
-        <v>0</v>
-      </c>
-      <c r="BJ65">
-        <v>1</v>
+      <c r="AY65" s="3">
+        <v>0</v>
+      </c>
+      <c r="AZ65" s="9">
+        <v>15</v>
+      </c>
+      <c r="BA65" s="3">
+        <v>0</v>
+      </c>
+      <c r="BB65" s="3">
+        <v>240</v>
+      </c>
+      <c r="BC65" s="3">
+        <v>0</v>
+      </c>
+      <c r="BD65" s="13">
+        <v>255</v>
+      </c>
+      <c r="BE65" s="3">
+        <v>34</v>
+      </c>
+      <c r="BF65" s="3">
+        <v>158</v>
+      </c>
+      <c r="BG65" s="3">
+        <v>20</v>
+      </c>
+      <c r="BH65" s="3">
+        <v>16</v>
+      </c>
+      <c r="BI65" s="3">
+        <v>0</v>
+      </c>
+      <c r="BJ65" s="3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -12689,11 +12704,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -12707,21 +12722,21 @@
     <row r="1" spans="1:5" ht="27.75" customHeight="1">
       <c r="A1" s="7"/>
       <c r="B1" s="23" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B2" s="26">
         <v>8</v>
@@ -12738,7 +12753,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="24" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B3" s="27">
         <v>0</v>
@@ -12755,7 +12770,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="24" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B4" s="26">
         <v>11</v>
@@ -12772,7 +12787,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B5" s="27">
         <v>0</v>
@@ -12789,7 +12804,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="24" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B6" s="27">
         <v>0</v>
@@ -12806,7 +12821,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" s="27">
         <v>0</v>
@@ -12823,7 +12838,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8" s="27">
         <v>0</v>
@@ -12840,7 +12855,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="24" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B9" s="27">
         <v>0</v>
@@ -12857,7 +12872,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B10" s="28">
         <v>9</v>
@@ -12874,7 +12889,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B11" s="26">
         <v>10</v>
@@ -12891,7 +12906,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B12" s="26">
         <v>14</v>
@@ -12908,7 +12923,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="24" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B13" s="26">
         <v>12</v>
@@ -12925,7 +12940,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B14" s="28">
         <v>2</v>
@@ -12942,7 +12957,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="24" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B15" s="28">
         <v>19</v>
@@ -12959,7 +12974,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B16" s="28">
         <v>17</v>
@@ -12973,12 +12988,12 @@
         <v>1</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="24" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B17" s="28">
         <v>5</v>
@@ -12995,7 +13010,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="24" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B18" s="28">
         <v>17</v>
@@ -13009,12 +13024,12 @@
         <v>1</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="24" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B19" s="27">
         <v>0</v>
@@ -13031,7 +13046,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B20" s="28">
         <v>18</v>
@@ -13045,12 +13060,12 @@
         <v>1</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="24" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B21" s="28">
         <v>16</v>
@@ -13067,7 +13082,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="24" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B22" s="26">
         <v>30</v>
@@ -13084,7 +13099,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="24" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B23" s="26">
         <v>27</v>
@@ -13101,7 +13116,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="24" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B24" s="28">
         <v>17</v>
@@ -13115,12 +13130,12 @@
         <v>1</v>
       </c>
       <c r="E24" s="25" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B26" s="28">
         <v>25</v>
@@ -13161,13 +13176,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -13709,10 +13724,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C1" s="7"/>
     </row>

</xml_diff>